<commit_message>
Salesforce api changes refinement
</commit_message>
<xml_diff>
--- a/resources/TestDataSheet_UATEnvironment.xlsx
+++ b/resources/TestDataSheet_UATEnvironment.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58796B9D-1FCF-4F56-A7E1-079CDE87BB4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="216" windowWidth="22944" windowHeight="12024" activeTab="1"/>
+    <workbookView xWindow="96" yWindow="216" windowWidth="22944" windowHeight="12024" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="2" name="Global" state="visible" r:id="rId4"/>
-    <sheet sheetId="4" name="Salesforce" state="visible" r:id="rId5"/>
-    <sheet sheetId="5" name="Ecommerce" state="visible" r:id="rId6"/>
+    <sheet name="Global" sheetId="2" r:id="rId1"/>
+    <sheet name="Salesforce" sheetId="4" r:id="rId2"/>
+    <sheet name="Ecommerce" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>testCaseName</t>
   </si>
@@ -39,9 +40,6 @@
     <t>Test Opportunity Name</t>
   </si>
   <si>
-    <t>006dL000005q8ugQAA</t>
-  </si>
-  <si>
     <t>TC002_Salesforce_RegressionTest</t>
   </si>
   <si>
@@ -63,45 +61,45 @@
     <t>https://rahulshettyacademy.com</t>
   </si>
   <si>
-    <t>67375947ae2afd4c0bc0558f</t>
-  </si>
-  <si>
-    <t>67375947ae2afd4c0bc05593</t>
-  </si>
-  <si>
     <t>TC002_Ecommerce_RegressionTest</t>
   </si>
   <si>
     <t>TC003_Ecommerce_RegressionTest</t>
+  </si>
+  <si>
+    <t>AccountName</t>
+  </si>
+  <si>
+    <t>Adams25 Inc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <u/>
+      <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="4">
@@ -113,13 +111,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.3999755851924192"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.5999938962981048"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -452,21 +450,21 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.3" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.88671875" customWidth="1"/>
     <col min="2" max="2" width="44.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="28.8" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -482,26 +480,26 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="77" zoomScaleNormal="70">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView zoomScale="77" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.3" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="34.44140625" customWidth="1"/>
-    <col min="2" max="2" width="21.21875" customWidth="1"/>
-    <col min="3" max="3" width="18.77734375" customWidth="1"/>
+    <col min="2" max="3" width="21.21875" customWidth="1"/>
+    <col min="4" max="4" width="18.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -509,10 +507,13 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" ht="14.4" customHeight="1" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="5" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
@@ -520,42 +521,49 @@
         <v>6</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>8</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="7"/>
-    </row>
-    <row r="4" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="7"/>
+    </row>
+    <row r="4" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="7"/>
+      <c r="C4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.3" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="34.44140625" customWidth="1"/>
     <col min="2" max="2" width="28.5546875" customWidth="1"/>
@@ -568,45 +576,41 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" ht="14.4" customHeight="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>16</v>
-      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>

</xml_diff>